<commit_message>
remove brackets from role column values
</commit_message>
<xml_diff>
--- a/MilitaryAircraft/aircraft.xlsx
+++ b/MilitaryAircraft/aircraft.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="542">
   <si>
     <t>aircraft</t>
   </si>
@@ -97,7 +97,7 @@
     <t>C-145A Skytruck</t>
   </si>
   <si>
-    <t>C-146A Wolfhound</t>
+    <t>C-146A Wolfhound[8]</t>
   </si>
   <si>
     <t>CN-235</t>
@@ -118,7 +118,7 @@
     <t>E-9A Widget</t>
   </si>
   <si>
-    <t>E-11A (BACN)</t>
+    <t>E-11A (BACN)[10]</t>
   </si>
   <si>
     <t>EC-130H Compass Call</t>
@@ -772,7 +772,7 @@
     <t>Multi-mission/Special Operations</t>
   </si>
   <si>
-    <t>Multi-mission[13]</t>
+    <t>Multi-mission</t>
   </si>
   <si>
     <t>Test Bed</t>
@@ -824,9 +824,6 @@
   </si>
   <si>
     <t>Electronic-warfare</t>
-  </si>
-  <si>
-    <t>Multi-mission</t>
   </si>
   <si>
     <t>Medium Range Recovery (MRR)</t>
@@ -2058,16 +2055,16 @@
         <v>230</v>
       </c>
       <c r="F2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2087,19 +2084,19 @@
         <v>230</v>
       </c>
       <c r="F3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2119,19 +2116,19 @@
         <v>230</v>
       </c>
       <c r="F4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2151,19 +2148,19 @@
         <v>231</v>
       </c>
       <c r="F5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2183,19 +2180,19 @@
         <v>231</v>
       </c>
       <c r="F6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2215,19 +2212,19 @@
         <v>231</v>
       </c>
       <c r="F7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2247,16 +2244,16 @@
         <v>232</v>
       </c>
       <c r="F8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2276,19 +2273,19 @@
         <v>233</v>
       </c>
       <c r="F9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2308,19 +2305,19 @@
         <v>232</v>
       </c>
       <c r="F10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K10" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2340,16 +2337,16 @@
         <v>234</v>
       </c>
       <c r="F11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K11" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2369,16 +2366,16 @@
         <v>234</v>
       </c>
       <c r="F12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K12" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2398,16 +2395,16 @@
         <v>234</v>
       </c>
       <c r="F13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K13" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2427,16 +2424,16 @@
         <v>234</v>
       </c>
       <c r="F14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K14" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2456,16 +2453,16 @@
         <v>235</v>
       </c>
       <c r="F15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K15" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2485,16 +2482,16 @@
         <v>235</v>
       </c>
       <c r="F16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J16" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K16" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2514,19 +2511,19 @@
         <v>236</v>
       </c>
       <c r="F17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2546,19 +2543,19 @@
         <v>233</v>
       </c>
       <c r="F18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="K18" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -2578,19 +2575,19 @@
         <v>237</v>
       </c>
       <c r="F19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J19" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2610,16 +2607,16 @@
         <v>238</v>
       </c>
       <c r="F20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J20" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2639,16 +2636,16 @@
         <v>239</v>
       </c>
       <c r="F21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J21" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K21" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2668,19 +2665,19 @@
         <v>240</v>
       </c>
       <c r="F22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J22" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K22" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2700,16 +2697,16 @@
         <v>240</v>
       </c>
       <c r="F23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G23" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J23" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K23" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -2729,16 +2726,16 @@
         <v>241</v>
       </c>
       <c r="F24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J24" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K24" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2758,16 +2755,16 @@
         <v>242</v>
       </c>
       <c r="F25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J25" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K25" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2787,16 +2784,16 @@
         <v>243</v>
       </c>
       <c r="F26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K26" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2816,16 +2813,16 @@
         <v>243</v>
       </c>
       <c r="F27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J27" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K27" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2845,22 +2842,22 @@
         <v>244</v>
       </c>
       <c r="F28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I28" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K28" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2880,16 +2877,16 @@
         <v>245</v>
       </c>
       <c r="F29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K29" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2909,19 +2906,19 @@
         <v>245</v>
       </c>
       <c r="F30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J30" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K30" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2941,22 +2938,22 @@
         <v>246</v>
       </c>
       <c r="F31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H31" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I31" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J31" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K31" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2976,19 +2973,19 @@
         <v>244</v>
       </c>
       <c r="F32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I32" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J32" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K32" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -3008,19 +3005,19 @@
         <v>246</v>
       </c>
       <c r="F33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J33" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K33" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -3040,16 +3037,16 @@
         <v>247</v>
       </c>
       <c r="F34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J34" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K34" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -3069,19 +3066,19 @@
         <v>248</v>
       </c>
       <c r="F35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I35" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J35" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K35" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -3101,16 +3098,16 @@
         <v>249</v>
       </c>
       <c r="F36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G36" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J36" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K36" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -3130,19 +3127,19 @@
         <v>249</v>
       </c>
       <c r="F37" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G37" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I37" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J37" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K37" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -3162,16 +3159,16 @@
         <v>249</v>
       </c>
       <c r="F38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J38" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K38" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -3191,19 +3188,19 @@
         <v>250</v>
       </c>
       <c r="F39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G39" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I39" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J39" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K39" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -3223,16 +3220,16 @@
         <v>251</v>
       </c>
       <c r="F40" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G40" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J40" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K40" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -3252,16 +3249,16 @@
         <v>251</v>
       </c>
       <c r="F41" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J41" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K41" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -3281,16 +3278,16 @@
         <v>252</v>
       </c>
       <c r="F42" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="K42" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -3310,16 +3307,16 @@
         <v>253</v>
       </c>
       <c r="F43" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G43" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J43" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K43" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -3339,19 +3336,19 @@
         <v>254</v>
       </c>
       <c r="F44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G44" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I44" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J44" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K44" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -3371,19 +3368,19 @@
         <v>237</v>
       </c>
       <c r="F45" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I45" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J45" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K45" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -3403,16 +3400,16 @@
         <v>237</v>
       </c>
       <c r="F46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G46" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J46" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K46" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -3432,16 +3429,16 @@
         <v>255</v>
       </c>
       <c r="F47" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G47" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J47" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K47" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -3461,16 +3458,16 @@
         <v>256</v>
       </c>
       <c r="F48" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J48" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K48" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -3490,16 +3487,16 @@
         <v>256</v>
       </c>
       <c r="F49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G49" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H49" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K49" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -3519,16 +3516,16 @@
         <v>257</v>
       </c>
       <c r="F50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H50" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K50" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -3548,19 +3545,19 @@
         <v>258</v>
       </c>
       <c r="F51" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G51" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I51" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J51" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K51" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -3580,16 +3577,16 @@
         <v>258</v>
       </c>
       <c r="F52" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G52" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J52" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K52" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -3609,16 +3606,16 @@
         <v>258</v>
       </c>
       <c r="F53" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G53" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J53" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K53" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -3638,16 +3635,16 @@
         <v>259</v>
       </c>
       <c r="F54" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G54" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J54" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K54" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -3667,16 +3664,16 @@
         <v>259</v>
       </c>
       <c r="F55" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G55" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J55" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K55" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -3696,16 +3693,16 @@
         <v>259</v>
       </c>
       <c r="F56" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G56" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J56" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K56" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -3725,16 +3722,16 @@
         <v>258</v>
       </c>
       <c r="F57" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G57" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J57" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K57" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -3754,16 +3751,16 @@
         <v>258</v>
       </c>
       <c r="F58" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G58" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J58" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K58" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -3783,16 +3780,16 @@
         <v>258</v>
       </c>
       <c r="F59" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G59" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J59" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K59" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -3812,16 +3809,16 @@
         <v>260</v>
       </c>
       <c r="F60" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G60" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J60" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K60" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -3841,16 +3838,16 @@
         <v>237</v>
       </c>
       <c r="F61" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G61" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J61" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K61" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3870,19 +3867,19 @@
         <v>236</v>
       </c>
       <c r="F62" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G62" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I62" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J62" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K62" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3902,19 +3899,19 @@
         <v>236</v>
       </c>
       <c r="F63" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G63" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I63" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J63" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K63" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3934,19 +3931,19 @@
         <v>236</v>
       </c>
       <c r="F64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I64" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J64" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K64" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -3966,19 +3963,19 @@
         <v>261</v>
       </c>
       <c r="F65" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G65" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I65" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J65" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K65" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -3998,19 +3995,19 @@
         <v>262</v>
       </c>
       <c r="F66" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I66" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J66" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K66" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -4030,16 +4027,16 @@
         <v>263</v>
       </c>
       <c r="F67" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G67" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J67" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K67" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -4059,22 +4056,22 @@
         <v>264</v>
       </c>
       <c r="F68" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H68">
         <v>2</v>
       </c>
       <c r="I68" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J68" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K68" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -4094,16 +4091,16 @@
         <v>233</v>
       </c>
       <c r="F69" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G69" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J69" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K69" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -4123,19 +4120,19 @@
         <v>265</v>
       </c>
       <c r="F70" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G70" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I70" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J70" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K70" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -4155,16 +4152,16 @@
         <v>265</v>
       </c>
       <c r="F71" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G71" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J71" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K71" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -4184,16 +4181,16 @@
         <v>265</v>
       </c>
       <c r="F72" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G72" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J72" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K72" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -4213,19 +4210,19 @@
         <v>250</v>
       </c>
       <c r="F73" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G73" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I73" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J73" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K73" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -4245,19 +4242,19 @@
         <v>265</v>
       </c>
       <c r="F74" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G74" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I74" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J74" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K74" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -4277,16 +4274,16 @@
         <v>261</v>
       </c>
       <c r="F75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J75" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K75" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -4306,19 +4303,19 @@
         <v>266</v>
       </c>
       <c r="F76" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G76" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I76" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J76" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="K76" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -4338,19 +4335,19 @@
         <v>237</v>
       </c>
       <c r="F77" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G77" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I77" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J77" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K77" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -4370,19 +4367,19 @@
         <v>267</v>
       </c>
       <c r="F78" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G78" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I78" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J78" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K78" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -4402,19 +4399,19 @@
         <v>261</v>
       </c>
       <c r="F79" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G79" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I79" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J79" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K79" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -4434,19 +4431,19 @@
         <v>256</v>
       </c>
       <c r="F80" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G80" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I80" t="s">
         <v>264</v>
       </c>
       <c r="J80" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K80" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -4466,19 +4463,19 @@
         <v>265</v>
       </c>
       <c r="F81" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G81" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J81" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K81" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -4498,16 +4495,16 @@
         <v>268</v>
       </c>
       <c r="F82" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G82" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J82" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K82" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -4527,19 +4524,19 @@
         <v>268</v>
       </c>
       <c r="F83" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G83" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I83" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J83" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="K83" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -4559,19 +4556,19 @@
         <v>233</v>
       </c>
       <c r="F84" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G84" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I84" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J84" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K84" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -4591,16 +4588,16 @@
         <v>269</v>
       </c>
       <c r="F85" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G85" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J85" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K85" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -4617,22 +4614,22 @@
         <v>229</v>
       </c>
       <c r="E86" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="F86" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G86" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I86" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J86" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K86" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -4649,22 +4646,22 @@
         <v>229</v>
       </c>
       <c r="E87" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="F87" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G87" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I87" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J87" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="K87" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -4684,19 +4681,19 @@
         <v>236</v>
       </c>
       <c r="F88" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G88" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I88" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J88" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K88" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -4716,19 +4713,19 @@
         <v>236</v>
       </c>
       <c r="F89" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G89" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I89" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J89" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K89" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -4745,19 +4742,19 @@
         <v>227</v>
       </c>
       <c r="F90" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G90" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I90" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J90" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K90" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -4774,19 +4771,19 @@
         <v>227</v>
       </c>
       <c r="F91" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G91" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I91" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J91" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K91" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -4806,19 +4803,19 @@
         <v>233</v>
       </c>
       <c r="F92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G92" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I92" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J92" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K92" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -4835,19 +4832,19 @@
         <v>227</v>
       </c>
       <c r="F93" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G93" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I93" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J93" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="K93" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -4864,13 +4861,13 @@
         <v>227</v>
       </c>
       <c r="F94" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G94" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K94" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -4890,13 +4887,13 @@
         <v>256</v>
       </c>
       <c r="F95" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G95" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K95" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -4916,19 +4913,19 @@
         <v>247</v>
       </c>
       <c r="F96" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G96" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I96" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J96" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K96" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -4948,19 +4945,19 @@
         <v>234</v>
       </c>
       <c r="F97" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G97" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I97" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J97" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K97" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -4980,19 +4977,19 @@
         <v>234</v>
       </c>
       <c r="F98" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G98" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I98" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J98" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K98" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -5012,19 +5009,19 @@
         <v>247</v>
       </c>
       <c r="F99" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G99" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I99" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J99" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K99" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -5044,19 +5041,19 @@
         <v>247</v>
       </c>
       <c r="F100" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G100" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I100" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J100" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K100" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -5076,16 +5073,16 @@
         <v>247</v>
       </c>
       <c r="F101" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G101" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J101" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K101" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="102" spans="1:11">
@@ -5105,19 +5102,19 @@
         <v>247</v>
       </c>
       <c r="F102" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G102" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I102" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J102" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K102" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -5134,22 +5131,22 @@
         <v>229</v>
       </c>
       <c r="E103" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F103" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G103" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I103" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J103" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K103" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -5166,19 +5163,19 @@
         <v>229</v>
       </c>
       <c r="E104" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F104" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G104" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J104" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K104" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -5195,22 +5192,22 @@
         <v>229</v>
       </c>
       <c r="E105" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F105" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G105" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I105" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J105" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K105" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="106" spans="1:11">
@@ -5227,25 +5224,25 @@
         <v>226</v>
       </c>
       <c r="E106" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F106" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G106" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H106">
         <v>2</v>
       </c>
       <c r="I106" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J106" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K106" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -5262,25 +5259,25 @@
         <v>226</v>
       </c>
       <c r="E107" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F107" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G107" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H107">
         <v>55</v>
       </c>
       <c r="I107" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J107" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K107" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -5297,25 +5294,25 @@
         <v>226</v>
       </c>
       <c r="E108" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F108" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G108" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H108">
         <v>7</v>
       </c>
       <c r="I108" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J108" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K108" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="109" spans="1:11">
@@ -5332,25 +5329,25 @@
         <v>226</v>
       </c>
       <c r="E109" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F109" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G109" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H109">
         <v>119</v>
       </c>
       <c r="I109" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J109" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K109" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="110" spans="1:11">
@@ -5367,25 +5364,25 @@
         <v>226</v>
       </c>
       <c r="E110" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F110" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G110" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H110">
         <v>92</v>
       </c>
       <c r="I110" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J110" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K110" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="111" spans="1:11">
@@ -5402,25 +5399,25 @@
         <v>226</v>
       </c>
       <c r="E111" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F111" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G111" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H111">
         <v>57</v>
       </c>
       <c r="I111" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J111" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K111" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -5437,22 +5434,22 @@
         <v>226</v>
       </c>
       <c r="E112" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F112" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G112" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I112" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J112" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K112" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="113" spans="1:11">
@@ -5472,16 +5469,16 @@
         <v>249</v>
       </c>
       <c r="F113" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G113" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J113" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K113" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="114" spans="1:11">
@@ -5501,22 +5498,22 @@
         <v>236</v>
       </c>
       <c r="F114" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G114" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H114">
         <v>8</v>
       </c>
       <c r="I114" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J114" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K114" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="115" spans="1:11">
@@ -5536,22 +5533,22 @@
         <v>236</v>
       </c>
       <c r="F115" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G115" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H115">
         <v>2</v>
       </c>
       <c r="I115" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J115" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K115" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="116" spans="1:11">
@@ -5571,22 +5568,22 @@
         <v>236</v>
       </c>
       <c r="F116" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G116" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H116">
         <v>4</v>
       </c>
       <c r="I116" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J116" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K116" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="117" spans="1:11">
@@ -5606,22 +5603,22 @@
         <v>236</v>
       </c>
       <c r="F117" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G117" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H117">
         <v>10</v>
       </c>
       <c r="I117" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J117" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="K117" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="118" spans="1:11">
@@ -5641,22 +5638,22 @@
         <v>236</v>
       </c>
       <c r="F118" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G118" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H118">
         <v>2</v>
       </c>
       <c r="I118" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J118" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K118" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="119" spans="1:11">
@@ -5676,19 +5673,19 @@
         <v>268</v>
       </c>
       <c r="F119" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G119" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I119" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J119" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="K119" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -5708,22 +5705,22 @@
         <v>265</v>
       </c>
       <c r="F120" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G120" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H120">
         <v>142</v>
       </c>
       <c r="I120" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J120" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K120" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="121" spans="1:11">
@@ -5743,19 +5740,19 @@
         <v>236</v>
       </c>
       <c r="F121" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G121" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H121">
         <v>160</v>
       </c>
       <c r="J121" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K121" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="122" spans="1:11">
@@ -5772,22 +5769,22 @@
         <v>229</v>
       </c>
       <c r="E122" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F122" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G122" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I122" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J122" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K122" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="123" spans="1:11">
@@ -5804,22 +5801,22 @@
         <v>229</v>
       </c>
       <c r="E123" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F123" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G123" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I123" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J123" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K123" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="124" spans="1:11">
@@ -5836,25 +5833,25 @@
         <v>226</v>
       </c>
       <c r="E124" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F124" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G124" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H124">
         <v>97</v>
       </c>
       <c r="I124" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J124" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K124" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="125" spans="1:11">
@@ -5871,25 +5868,25 @@
         <v>228</v>
       </c>
       <c r="E125" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="F125" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G125" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H125">
         <v>300</v>
       </c>
       <c r="I125" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J125" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K125" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="126" spans="1:11">
@@ -5906,22 +5903,22 @@
         <v>229</v>
       </c>
       <c r="E126" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F126" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G126" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I126" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J126" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K126" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="127" spans="1:11">
@@ -5941,16 +5938,16 @@
         <v>237</v>
       </c>
       <c r="F127" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G127" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J127" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K127" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="128" spans="1:11">
@@ -5970,13 +5967,13 @@
         <v>237</v>
       </c>
       <c r="F128" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G128" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K128" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="129" spans="1:11">
@@ -5996,13 +5993,13 @@
         <v>237</v>
       </c>
       <c r="F129" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G129" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K129" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="130" spans="1:11">
@@ -6022,13 +6019,13 @@
         <v>237</v>
       </c>
       <c r="F130" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G130" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K130" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="131" spans="1:11">
@@ -6048,13 +6045,13 @@
         <v>237</v>
       </c>
       <c r="F131" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G131" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K131" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="132" spans="1:11">
@@ -6074,16 +6071,16 @@
         <v>257</v>
       </c>
       <c r="F132" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G132" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J132" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K132" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="133" spans="1:11">
@@ -6100,13 +6097,13 @@
         <v>229</v>
       </c>
       <c r="F133" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G133" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K133" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="134" spans="1:11">
@@ -6123,22 +6120,22 @@
         <v>227</v>
       </c>
       <c r="E134" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F134" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G134" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I134" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J134" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K134" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="135" spans="1:11">
@@ -6155,22 +6152,22 @@
         <v>226</v>
       </c>
       <c r="E135" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F135" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G135" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I135" t="s">
         <v>114</v>
       </c>
       <c r="J135" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K135" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="136" spans="1:11">
@@ -6187,22 +6184,22 @@
         <v>226</v>
       </c>
       <c r="E136" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F136" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G136" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I136" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J136" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K136" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="137" spans="1:11">
@@ -6219,19 +6216,19 @@
         <v>226</v>
       </c>
       <c r="E137" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F137" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G137" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J137" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K137" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="138" spans="1:11">
@@ -6248,19 +6245,19 @@
         <v>227</v>
       </c>
       <c r="E138" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F138" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G138" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J138" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K138" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="139" spans="1:11">
@@ -6277,19 +6274,19 @@
         <v>227</v>
       </c>
       <c r="E139" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F139" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G139" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J139" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="K139" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="140" spans="1:11">
@@ -6306,19 +6303,19 @@
         <v>227</v>
       </c>
       <c r="E140" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F140" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G140" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J140" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K140" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="141" spans="1:11">
@@ -6335,19 +6332,19 @@
         <v>227</v>
       </c>
       <c r="E141" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F141" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G141" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J141" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K141" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="142" spans="1:11">
@@ -6364,19 +6361,19 @@
         <v>227</v>
       </c>
       <c r="E142" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F142" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G142" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J142" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="K142" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="143" spans="1:11">
@@ -6393,19 +6390,19 @@
         <v>226</v>
       </c>
       <c r="E143" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F143" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G143" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J143" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K143" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="144" spans="1:11">
@@ -6422,19 +6419,19 @@
         <v>226</v>
       </c>
       <c r="E144" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F144" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G144" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J144" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="K144" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="145" spans="1:11">
@@ -6451,19 +6448,19 @@
         <v>227</v>
       </c>
       <c r="E145" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F145" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G145" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J145" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K145" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="146" spans="1:11">
@@ -6480,22 +6477,22 @@
         <v>226</v>
       </c>
       <c r="E146" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F146" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G146" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I146" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J146" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K146" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="147" spans="1:11">
@@ -6512,22 +6509,22 @@
         <v>226</v>
       </c>
       <c r="E147" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F147" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G147" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I147" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J147" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="K147" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="148" spans="1:11">
@@ -6544,22 +6541,22 @@
         <v>226</v>
       </c>
       <c r="E148" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F148" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G148" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I148" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J148" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="K148" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="149" spans="1:11">
@@ -6576,22 +6573,22 @@
         <v>226</v>
       </c>
       <c r="E149" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F149" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G149" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I149" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J149" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="K149" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="150" spans="1:11">
@@ -6608,22 +6605,22 @@
         <v>226</v>
       </c>
       <c r="E150" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F150" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G150" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I150" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J150" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K150" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="151" spans="1:11">
@@ -6640,22 +6637,22 @@
         <v>227</v>
       </c>
       <c r="E151" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F151" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G151" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I151" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J151" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K151" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="152" spans="1:11">
@@ -6672,22 +6669,22 @@
         <v>226</v>
       </c>
       <c r="E152" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F152" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G152" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I152" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J152" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="K152" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="153" spans="1:11">
@@ -6704,22 +6701,22 @@
         <v>227</v>
       </c>
       <c r="E153" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F153" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G153" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I153" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J153" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="K153" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="154" spans="1:11">
@@ -6736,19 +6733,19 @@
         <v>227</v>
       </c>
       <c r="E154" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F154" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G154" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J154" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="K154" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="155" spans="1:11">
@@ -6765,19 +6762,19 @@
         <v>226</v>
       </c>
       <c r="E155" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F155" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G155" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J155" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K155" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="156" spans="1:11">
@@ -6797,16 +6794,16 @@
         <v>267</v>
       </c>
       <c r="F156" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G156" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J156" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K156" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="157" spans="1:11">
@@ -6823,22 +6820,22 @@
         <v>228</v>
       </c>
       <c r="E157" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="F157" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G157" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I157" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J157" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K157" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="158" spans="1:11">
@@ -6855,19 +6852,19 @@
         <v>229</v>
       </c>
       <c r="E158" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F158" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G158" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J158" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K158" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="159" spans="1:11">
@@ -6884,19 +6881,19 @@
         <v>229</v>
       </c>
       <c r="E159" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F159" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G159" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J159" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="K159" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="160" spans="1:11">
@@ -6916,19 +6913,19 @@
         <v>258</v>
       </c>
       <c r="F160" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G160" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I160" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J160" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="K160" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="161" spans="1:11">
@@ -6945,13 +6942,13 @@
         <v>227</v>
       </c>
       <c r="F161" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G161" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K161" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="162" spans="1:11">
@@ -6968,13 +6965,13 @@
         <v>227</v>
       </c>
       <c r="F162" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G162" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K162" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="163" spans="1:11">
@@ -6994,19 +6991,19 @@
         <v>256</v>
       </c>
       <c r="F163" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G163" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I163" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J163" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K163" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>